<commit_message>
added 15th March session
</commit_message>
<xml_diff>
--- a/data/savingSessions_dateTimes.xlsx
+++ b/data/savingSessions_dateTimes.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/repos/github/dataknut/savingSessions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9240CB54-E94D-834C-8AAB-D0BA8CF7EF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5273BDDB-C807-0F48-AC1F-020EE03F8833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FBB7DBF6-62CA-B543-B465-8D0D4DEE8528}"/>
   </bookViews>
   <sheets>
     <sheet name="dateTimes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -406,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C87E3B8-B7D4-A845-BFFE-A619B8961CEA}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -586,6 +586,20 @@
         <v>44978.75</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45000.770833333336</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45000.791666666664</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 23/3/23 saving session
</commit_message>
<xml_diff>
--- a/data/savingSessions_dateTimes.xlsx
+++ b/data/savingSessions_dateTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/repos/github/dataknut/savingSessions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5273BDDB-C807-0F48-AC1F-020EE03F8833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C7D5BA-E267-CC45-803B-55608DF737C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FBB7DBF6-62CA-B543-B465-8D0D4DEE8528}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C87E3B8-B7D4-A845-BFFE-A619B8961CEA}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,6 +600,20 @@
         <v>45000.791666666664</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45008.770833333336</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45008.791666666664</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>